<commit_message>
added more display settings to settings sheet
</commit_message>
<xml_diff>
--- a/wordle_doc.xlsx
+++ b/wordle_doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Documents\GitHub\wordler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF374F4-14B6-4833-87A6-691FAB480C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2625C1-E696-4BF2-ABC2-156E481C9227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2919" uniqueCount="2320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2924" uniqueCount="2325">
   <si>
     <t>Date</t>
   </si>
@@ -6984,6 +6984,21 @@
   </si>
   <si>
     <t>Selection</t>
+  </si>
+  <si>
+    <t>Display number of words left?</t>
+  </si>
+  <si>
+    <t>Display remaining words?</t>
+  </si>
+  <si>
+    <t>Display guesses?</t>
+  </si>
+  <si>
+    <t>Display victory text?</t>
+  </si>
+  <si>
+    <t>Display word of the day?</t>
   </si>
 </sst>
 </file>
@@ -7399,9 +7414,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C6230C-193A-4FD4-8C52-C060F6680339}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7421,7 +7438,7 @@
         <v>2315</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7438,6 +7455,46 @@
       </c>
       <c r="B4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2320</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2321</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2324</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2323</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "added more display settings to settings sheet"
This reverts commit a39e2c55dde62bfcc63c55a2c5234e6bae14ae91.
</commit_message>
<xml_diff>
--- a/wordle_doc.xlsx
+++ b/wordle_doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Documents\GitHub\wordler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2625C1-E696-4BF2-ABC2-156E481C9227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF374F4-14B6-4833-87A6-691FAB480C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2924" uniqueCount="2325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2919" uniqueCount="2320">
   <si>
     <t>Date</t>
   </si>
@@ -6984,21 +6984,6 @@
   </si>
   <si>
     <t>Selection</t>
-  </si>
-  <si>
-    <t>Display number of words left?</t>
-  </si>
-  <si>
-    <t>Display remaining words?</t>
-  </si>
-  <si>
-    <t>Display guesses?</t>
-  </si>
-  <si>
-    <t>Display victory text?</t>
-  </si>
-  <si>
-    <t>Display word of the day?</t>
   </si>
 </sst>
 </file>
@@ -7414,11 +7399,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C6230C-193A-4FD4-8C52-C060F6680339}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7438,7 +7421,7 @@
         <v>2315</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7455,46 +7438,6 @@
       </c>
       <c r="B4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2320</v>
-      </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2321</v>
-      </c>
-      <c r="B6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>2322</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>2324</v>
-      </c>
-      <c r="B8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>2323</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran code a few times so updated excel sheet
</commit_message>
<xml_diff>
--- a/wordle_doc.xlsx
+++ b/wordle_doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-1395" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Performance Stats" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Config" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Guessing Path" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Past Words" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="All Guess Candidates" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Performance Stats" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Config" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Guessing Path" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Past Words" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="All Guess Candidates" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -429,10 +429,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -524,6 +524,51 @@
         <v>4</v>
       </c>
       <c r="C6" t="inlineStr">
+        <is>
+          <t>RAISE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-01-25</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>RAISE</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-01-26</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>RAISE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-01-27</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>RAISE</t>
         </is>
@@ -543,7 +588,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -606,10 +651,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -745,6 +790,72 @@
       <c r="E5" t="inlineStr">
         <is>
           <t>COUNT</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-01-25</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RAISE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MAIZE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-01-26</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>RAISE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>HEFTY</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>BEEFY</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-01-27</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>RAISE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>MORPH</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>LORRY</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>WORRY</t>
         </is>
       </c>
     </row>
@@ -759,10 +870,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A586"/>
+  <dimension ref="A1:A589"/>
   <sheetViews>
-    <sheetView topLeftCell="A581" workbookViewId="0">
-      <selection activeCell="A585" sqref="A585"/>
+    <sheetView tabSelected="1" topLeftCell="A581" workbookViewId="0">
+      <selection activeCell="B586" sqref="B586"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -4866,6 +4977,27 @@
       <c r="A586" t="inlineStr">
         <is>
           <t>COUNT</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>MAIZE</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>BEEFY</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>WORRY</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updates to past words and record keeping
</commit_message>
<xml_diff>
--- a/wordle_doc.xlsx
+++ b/wordle_doc.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -569,6 +569,21 @@
         <v>4</v>
       </c>
       <c r="C9" t="inlineStr">
+        <is>
+          <t>RAISE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-01-28</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>RAISE</t>
         </is>
@@ -651,7 +666,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -859,6 +874,28 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-01-28</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>RAISE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>FRILL</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>FLIRT</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -870,7 +907,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A589"/>
+  <dimension ref="A1:A590"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A581" workbookViewId="0">
       <selection activeCell="B586" sqref="B586"/>
@@ -4998,6 +5035,13 @@
       <c r="A589" t="inlineStr">
         <is>
           <t>WORRY</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>FLIRT</t>
         </is>
       </c>
     </row>

</xml_diff>